<commit_message>
Added creating a basic heatmap with some open crime data
</commit_message>
<xml_diff>
--- a/Data/CasesByZIPCode.xlsx
+++ b/Data/CasesByZIPCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandaclark/SoftwareProjects/Mapping/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78A7230-F91B-E843-B76F-123E0F72841F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{847D7148-040A-FD47-81B9-235F5631C7C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4662,11 +4662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:E430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A380" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B430"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4727,7 +4726,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -4741,7 +4740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1">
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -4755,7 +4754,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1">
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -4769,7 +4768,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1">
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -4783,7 +4782,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1">
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -4797,7 +4796,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1">
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -4811,7 +4810,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1">
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -4825,7 +4824,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1">
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
@@ -4856,7 +4855,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1">
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
@@ -4870,7 +4869,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1">
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
@@ -4884,7 +4883,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1">
+    <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
         <v>49</v>
       </c>
@@ -4898,7 +4897,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1">
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>53</v>
       </c>
@@ -4912,7 +4911,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1">
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>57</v>
       </c>
@@ -4926,7 +4925,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1">
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>61</v>
       </c>
@@ -4940,7 +4939,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1">
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
         <v>65</v>
       </c>
@@ -4971,7 +4970,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1">
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>71</v>
       </c>
@@ -4985,7 +4984,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1">
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
         <v>75</v>
       </c>
@@ -4999,7 +4998,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:5" hidden="1">
+    <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
         <v>79</v>
       </c>
@@ -5013,7 +5012,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:5" hidden="1">
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
         <v>83</v>
       </c>
@@ -5027,7 +5026,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:5" hidden="1">
+    <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
         <v>87</v>
       </c>
@@ -5041,7 +5040,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:5" hidden="1">
+    <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
         <v>91</v>
       </c>
@@ -5089,7 +5088,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="29" spans="1:5" hidden="1">
+    <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
         <v>99</v>
       </c>
@@ -5103,7 +5102,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:5" hidden="1">
+    <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
         <v>103</v>
       </c>
@@ -5117,7 +5116,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:5" hidden="1">
+    <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
         <v>107</v>
       </c>
@@ -5148,7 +5147,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="33" spans="1:5" hidden="1">
+    <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
         <v>113</v>
       </c>
@@ -5162,7 +5161,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:5" hidden="1">
+    <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
         <v>117</v>
       </c>
@@ -5193,7 +5192,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="36" spans="1:5" hidden="1">
+    <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
         <v>123</v>
       </c>
@@ -5224,7 +5223,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="38" spans="1:5" hidden="1">
+    <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
         <v>129</v>
       </c>
@@ -5238,7 +5237,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="39" spans="1:5" hidden="1">
+    <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
         <v>133</v>
       </c>
@@ -5252,7 +5251,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="1:5" hidden="1">
+    <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
         <v>137</v>
       </c>
@@ -5266,7 +5265,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:5" hidden="1">
+    <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
         <v>141</v>
       </c>
@@ -5280,7 +5279,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="42" spans="1:5" hidden="1">
+    <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
         <v>145</v>
       </c>
@@ -5294,7 +5293,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="43" spans="1:5" hidden="1">
+    <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
         <v>149</v>
       </c>
@@ -5325,7 +5324,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="45" spans="1:5" hidden="1">
+    <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
         <v>155</v>
       </c>
@@ -5339,7 +5338,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="46" spans="1:5" hidden="1">
+    <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
         <v>159</v>
       </c>
@@ -5353,7 +5352,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="47" spans="1:5" hidden="1">
+    <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
         <v>163</v>
       </c>
@@ -5367,7 +5366,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="48" spans="1:5" hidden="1">
+    <row r="48" spans="1:5">
       <c r="A48" s="1" t="s">
         <v>167</v>
       </c>
@@ -5381,7 +5380,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1">
+    <row r="49" spans="1:5">
       <c r="A49" s="1" t="s">
         <v>171</v>
       </c>
@@ -5412,7 +5411,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1">
+    <row r="51" spans="1:5">
       <c r="A51" s="1" t="s">
         <v>177</v>
       </c>
@@ -5426,7 +5425,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1">
+    <row r="52" spans="1:5">
       <c r="A52" s="1" t="s">
         <v>181</v>
       </c>
@@ -5440,7 +5439,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1">
+    <row r="53" spans="1:5">
       <c r="A53" s="1" t="s">
         <v>185</v>
       </c>
@@ -5454,7 +5453,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1">
+    <row r="54" spans="1:5">
       <c r="A54" s="1" t="s">
         <v>189</v>
       </c>
@@ -5468,7 +5467,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1">
+    <row r="55" spans="1:5">
       <c r="A55" s="1" t="s">
         <v>193</v>
       </c>
@@ -5499,7 +5498,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1">
+    <row r="57" spans="1:5">
       <c r="A57" s="1" t="s">
         <v>199</v>
       </c>
@@ -5513,7 +5512,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1">
+    <row r="58" spans="1:5">
       <c r="A58" s="1" t="s">
         <v>203</v>
       </c>
@@ -5527,7 +5526,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1">
+    <row r="59" spans="1:5">
       <c r="A59" s="1" t="s">
         <v>207</v>
       </c>
@@ -5541,7 +5540,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1">
+    <row r="60" spans="1:5">
       <c r="A60" s="1" t="s">
         <v>211</v>
       </c>
@@ -5555,7 +5554,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1">
+    <row r="61" spans="1:5">
       <c r="A61" s="1" t="s">
         <v>215</v>
       </c>
@@ -5569,7 +5568,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1">
+    <row r="62" spans="1:5">
       <c r="A62" s="1" t="s">
         <v>219</v>
       </c>
@@ -5583,7 +5582,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1">
+    <row r="63" spans="1:5">
       <c r="A63" s="1" t="s">
         <v>223</v>
       </c>
@@ -5597,7 +5596,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1">
+    <row r="64" spans="1:5">
       <c r="A64" s="1" t="s">
         <v>227</v>
       </c>
@@ -5611,7 +5610,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1">
+    <row r="65" spans="1:5">
       <c r="A65" s="1" t="s">
         <v>231</v>
       </c>
@@ -5642,7 +5641,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1">
+    <row r="67" spans="1:5">
       <c r="A67" s="1" t="s">
         <v>237</v>
       </c>
@@ -5656,7 +5655,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1">
+    <row r="68" spans="1:5">
       <c r="A68" s="1" t="s">
         <v>241</v>
       </c>
@@ -5670,7 +5669,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1">
+    <row r="69" spans="1:5">
       <c r="A69" s="1" t="s">
         <v>245</v>
       </c>
@@ -5718,7 +5717,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1">
+    <row r="72" spans="1:5">
       <c r="A72" s="1" t="s">
         <v>253</v>
       </c>
@@ -5732,7 +5731,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1">
+    <row r="73" spans="1:5">
       <c r="A73" s="1" t="s">
         <v>257</v>
       </c>
@@ -5746,7 +5745,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1">
+    <row r="74" spans="1:5">
       <c r="A74" s="1" t="s">
         <v>261</v>
       </c>
@@ -5760,7 +5759,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1">
+    <row r="75" spans="1:5">
       <c r="A75" s="1" t="s">
         <v>265</v>
       </c>
@@ -5774,7 +5773,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1">
+    <row r="76" spans="1:5">
       <c r="A76" s="1" t="s">
         <v>269</v>
       </c>
@@ -5788,7 +5787,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1">
+    <row r="77" spans="1:5">
       <c r="A77" s="1" t="s">
         <v>273</v>
       </c>
@@ -5802,7 +5801,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1">
+    <row r="78" spans="1:5">
       <c r="A78" s="1" t="s">
         <v>277</v>
       </c>
@@ -5850,7 +5849,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1">
+    <row r="81" spans="1:5">
       <c r="A81" s="1" t="s">
         <v>285</v>
       </c>
@@ -5864,7 +5863,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1">
+    <row r="82" spans="1:5">
       <c r="A82" s="1" t="s">
         <v>289</v>
       </c>
@@ -5895,7 +5894,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1">
+    <row r="84" spans="1:5">
       <c r="A84" s="1" t="s">
         <v>295</v>
       </c>
@@ -5909,7 +5908,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1">
+    <row r="85" spans="1:5">
       <c r="A85" s="1" t="s">
         <v>299</v>
       </c>
@@ -5940,7 +5939,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1">
+    <row r="87" spans="1:5">
       <c r="A87" s="1" t="s">
         <v>305</v>
       </c>
@@ -5954,7 +5953,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1">
+    <row r="88" spans="1:5">
       <c r="A88" s="1" t="s">
         <v>309</v>
       </c>
@@ -5985,7 +5984,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1">
+    <row r="90" spans="1:5">
       <c r="A90" s="1" t="s">
         <v>315</v>
       </c>
@@ -5999,7 +5998,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1">
+    <row r="91" spans="1:5">
       <c r="A91" s="1" t="s">
         <v>319</v>
       </c>
@@ -6013,7 +6012,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1">
+    <row r="92" spans="1:5">
       <c r="A92" s="1" t="s">
         <v>323</v>
       </c>
@@ -6061,7 +6060,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1">
+    <row r="95" spans="1:5">
       <c r="A95" s="1" t="s">
         <v>331</v>
       </c>
@@ -6075,7 +6074,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1">
+    <row r="96" spans="1:5">
       <c r="A96" s="1" t="s">
         <v>335</v>
       </c>
@@ -6089,7 +6088,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1">
+    <row r="97" spans="1:5">
       <c r="A97" s="1" t="s">
         <v>339</v>
       </c>
@@ -6103,7 +6102,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1">
+    <row r="98" spans="1:5">
       <c r="A98" s="1" t="s">
         <v>343</v>
       </c>
@@ -6117,7 +6116,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="99" spans="1:5" hidden="1">
+    <row r="99" spans="1:5">
       <c r="A99" s="1" t="s">
         <v>347</v>
       </c>
@@ -6165,7 +6164,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1">
+    <row r="102" spans="1:5">
       <c r="A102" s="1" t="s">
         <v>355</v>
       </c>
@@ -6196,7 +6195,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="104" spans="1:5" hidden="1">
+    <row r="104" spans="1:5">
       <c r="A104" s="1" t="s">
         <v>361</v>
       </c>
@@ -6227,7 +6226,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1">
+    <row r="106" spans="1:5">
       <c r="A106" s="1" t="s">
         <v>367</v>
       </c>
@@ -6241,7 +6240,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1">
+    <row r="107" spans="1:5">
       <c r="A107" s="1" t="s">
         <v>371</v>
       </c>
@@ -6255,7 +6254,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1">
+    <row r="108" spans="1:5">
       <c r="A108" s="1" t="s">
         <v>375</v>
       </c>
@@ -6269,7 +6268,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1">
+    <row r="109" spans="1:5">
       <c r="A109" s="1" t="s">
         <v>379</v>
       </c>
@@ -6283,7 +6282,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1">
+    <row r="110" spans="1:5">
       <c r="A110" s="1" t="s">
         <v>383</v>
       </c>
@@ -6297,7 +6296,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="111" spans="1:5" hidden="1">
+    <row r="111" spans="1:5">
       <c r="A111" s="1" t="s">
         <v>387</v>
       </c>
@@ -6328,7 +6327,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="113" spans="1:4" hidden="1">
+    <row r="113" spans="1:4">
       <c r="A113" s="1" t="s">
         <v>393</v>
       </c>
@@ -6342,7 +6341,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="114" spans="1:4" hidden="1">
+    <row r="114" spans="1:4">
       <c r="A114" s="1" t="s">
         <v>397</v>
       </c>
@@ -6356,7 +6355,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="115" spans="1:4" hidden="1">
+    <row r="115" spans="1:4">
       <c r="A115" s="1" t="s">
         <v>401</v>
       </c>
@@ -6370,7 +6369,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="116" spans="1:4" hidden="1">
+    <row r="116" spans="1:4">
       <c r="A116" s="1" t="s">
         <v>405</v>
       </c>
@@ -6384,7 +6383,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="117" spans="1:4" hidden="1">
+    <row r="117" spans="1:4">
       <c r="A117" s="1" t="s">
         <v>409</v>
       </c>
@@ -6398,7 +6397,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="118" spans="1:4" hidden="1">
+    <row r="118" spans="1:4">
       <c r="A118" s="1" t="s">
         <v>413</v>
       </c>
@@ -6412,7 +6411,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="119" spans="1:4" hidden="1">
+    <row r="119" spans="1:4">
       <c r="A119" s="1" t="s">
         <v>417</v>
       </c>
@@ -6426,7 +6425,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="120" spans="1:4" hidden="1">
+    <row r="120" spans="1:4">
       <c r="A120" s="1" t="s">
         <v>421</v>
       </c>
@@ -6440,7 +6439,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="121" spans="1:4" hidden="1">
+    <row r="121" spans="1:4">
       <c r="A121" s="1" t="s">
         <v>425</v>
       </c>
@@ -6454,7 +6453,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="122" spans="1:4" hidden="1">
+    <row r="122" spans="1:4">
       <c r="A122" s="1" t="s">
         <v>429</v>
       </c>
@@ -6468,7 +6467,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="123" spans="1:4" hidden="1">
+    <row r="123" spans="1:4">
       <c r="A123" s="1" t="s">
         <v>433</v>
       </c>
@@ -6482,7 +6481,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="124" spans="1:4" hidden="1">
+    <row r="124" spans="1:4">
       <c r="A124" s="1" t="s">
         <v>437</v>
       </c>
@@ -6496,7 +6495,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="125" spans="1:4" hidden="1">
+    <row r="125" spans="1:4">
       <c r="A125" s="1" t="s">
         <v>441</v>
       </c>
@@ -6510,7 +6509,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="126" spans="1:4" hidden="1">
+    <row r="126" spans="1:4">
       <c r="A126" s="1" t="s">
         <v>445</v>
       </c>
@@ -6524,7 +6523,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="127" spans="1:4" hidden="1">
+    <row r="127" spans="1:4">
       <c r="A127" s="1" t="s">
         <v>449</v>
       </c>
@@ -6538,7 +6537,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="128" spans="1:4" hidden="1">
+    <row r="128" spans="1:4">
       <c r="A128" s="1" t="s">
         <v>453</v>
       </c>
@@ -6552,7 +6551,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1">
+    <row r="129" spans="1:5">
       <c r="A129" s="1" t="s">
         <v>457</v>
       </c>
@@ -6566,7 +6565,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="130" spans="1:5" hidden="1">
+    <row r="130" spans="1:5">
       <c r="A130" s="1" t="s">
         <v>461</v>
       </c>
@@ -6580,7 +6579,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1">
+    <row r="131" spans="1:5">
       <c r="A131" s="1" t="s">
         <v>465</v>
       </c>
@@ -6594,7 +6593,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="132" spans="1:5" hidden="1">
+    <row r="132" spans="1:5">
       <c r="A132" s="1" t="s">
         <v>469</v>
       </c>
@@ -6608,7 +6607,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="133" spans="1:5" hidden="1">
+    <row r="133" spans="1:5">
       <c r="A133" s="1" t="s">
         <v>473</v>
       </c>
@@ -6622,7 +6621,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="134" spans="1:5" hidden="1">
+    <row r="134" spans="1:5">
       <c r="A134" s="1" t="s">
         <v>477</v>
       </c>
@@ -6636,7 +6635,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="135" spans="1:5" hidden="1">
+    <row r="135" spans="1:5">
       <c r="A135" s="1" t="s">
         <v>481</v>
       </c>
@@ -6650,7 +6649,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="136" spans="1:5" hidden="1">
+    <row r="136" spans="1:5">
       <c r="A136" s="1" t="s">
         <v>485</v>
       </c>
@@ -6664,7 +6663,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="137" spans="1:5" hidden="1">
+    <row r="137" spans="1:5">
       <c r="A137" s="1" t="s">
         <v>489</v>
       </c>
@@ -6695,7 +6694,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1">
+    <row r="139" spans="1:5">
       <c r="A139" s="1" t="s">
         <v>495</v>
       </c>
@@ -6709,7 +6708,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1">
+    <row r="140" spans="1:5">
       <c r="A140" s="1" t="s">
         <v>499</v>
       </c>
@@ -6757,7 +6756,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="143" spans="1:5" hidden="1">
+    <row r="143" spans="1:5">
       <c r="A143" s="1" t="s">
         <v>507</v>
       </c>
@@ -6771,7 +6770,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="144" spans="1:5" hidden="1">
+    <row r="144" spans="1:5">
       <c r="A144" s="1" t="s">
         <v>511</v>
       </c>
@@ -6785,7 +6784,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1">
+    <row r="145" spans="1:5">
       <c r="A145" s="1" t="s">
         <v>515</v>
       </c>
@@ -6799,7 +6798,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="146" spans="1:5" hidden="1">
+    <row r="146" spans="1:5">
       <c r="A146" s="1" t="s">
         <v>519</v>
       </c>
@@ -6813,7 +6812,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="147" spans="1:5" hidden="1">
+    <row r="147" spans="1:5">
       <c r="A147" s="1" t="s">
         <v>523</v>
       </c>
@@ -6827,7 +6826,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="148" spans="1:5" hidden="1">
+    <row r="148" spans="1:5">
       <c r="A148" s="1" t="s">
         <v>527</v>
       </c>
@@ -6875,7 +6874,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="151" spans="1:5" hidden="1">
+    <row r="151" spans="1:5">
       <c r="A151" s="1" t="s">
         <v>535</v>
       </c>
@@ -6889,7 +6888,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="152" spans="1:5" hidden="1">
+    <row r="152" spans="1:5">
       <c r="A152" s="1" t="s">
         <v>539</v>
       </c>
@@ -6903,7 +6902,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="153" spans="1:5" hidden="1">
+    <row r="153" spans="1:5">
       <c r="A153" s="1" t="s">
         <v>543</v>
       </c>
@@ -6917,7 +6916,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1">
+    <row r="154" spans="1:5">
       <c r="A154" s="1" t="s">
         <v>547</v>
       </c>
@@ -6931,7 +6930,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1">
+    <row r="155" spans="1:5">
       <c r="A155" s="1" t="s">
         <v>551</v>
       </c>
@@ -6962,7 +6961,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="157" spans="1:5" hidden="1">
+    <row r="157" spans="1:5">
       <c r="A157" s="1" t="s">
         <v>557</v>
       </c>
@@ -6993,7 +6992,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="159" spans="1:5" hidden="1">
+    <row r="159" spans="1:5">
       <c r="A159" s="1" t="s">
         <v>563</v>
       </c>
@@ -7007,7 +7006,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="160" spans="1:5" hidden="1">
+    <row r="160" spans="1:5">
       <c r="A160" s="1" t="s">
         <v>567</v>
       </c>
@@ -7021,7 +7020,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="161" spans="1:5" hidden="1">
+    <row r="161" spans="1:5">
       <c r="A161" s="1" t="s">
         <v>571</v>
       </c>
@@ -7035,7 +7034,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="162" spans="1:5" hidden="1">
+    <row r="162" spans="1:5">
       <c r="A162" s="1" t="s">
         <v>575</v>
       </c>
@@ -7049,7 +7048,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="163" spans="1:5" hidden="1">
+    <row r="163" spans="1:5">
       <c r="A163" s="1" t="s">
         <v>579</v>
       </c>
@@ -7097,7 +7096,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="166" spans="1:5" hidden="1">
+    <row r="166" spans="1:5">
       <c r="A166" s="1" t="s">
         <v>587</v>
       </c>
@@ -7145,7 +7144,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="169" spans="1:5" hidden="1">
+    <row r="169" spans="1:5">
       <c r="A169" s="1" t="s">
         <v>595</v>
       </c>
@@ -7159,7 +7158,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="170" spans="1:5" hidden="1">
+    <row r="170" spans="1:5">
       <c r="A170" s="1" t="s">
         <v>599</v>
       </c>
@@ -7190,7 +7189,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="172" spans="1:5" hidden="1">
+    <row r="172" spans="1:5">
       <c r="A172" s="1" t="s">
         <v>605</v>
       </c>
@@ -7204,7 +7203,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="173" spans="1:5" hidden="1">
+    <row r="173" spans="1:5">
       <c r="A173" s="1" t="s">
         <v>609</v>
       </c>
@@ -7218,7 +7217,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="174" spans="1:5" hidden="1">
+    <row r="174" spans="1:5">
       <c r="A174" s="1" t="s">
         <v>613</v>
       </c>
@@ -7249,7 +7248,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="176" spans="1:5" hidden="1">
+    <row r="176" spans="1:5">
       <c r="A176" s="1" t="s">
         <v>619</v>
       </c>
@@ -7263,7 +7262,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="177" spans="1:5" hidden="1">
+    <row r="177" spans="1:5">
       <c r="A177" s="1" t="s">
         <v>623</v>
       </c>
@@ -7277,7 +7276,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="178" spans="1:5" hidden="1">
+    <row r="178" spans="1:5">
       <c r="A178" s="1" t="s">
         <v>627</v>
       </c>
@@ -7291,7 +7290,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="179" spans="1:5" hidden="1">
+    <row r="179" spans="1:5">
       <c r="A179" s="1" t="s">
         <v>631</v>
       </c>
@@ -7322,7 +7321,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="181" spans="1:5" hidden="1">
+    <row r="181" spans="1:5">
       <c r="A181" s="1" t="s">
         <v>637</v>
       </c>
@@ -7336,7 +7335,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="182" spans="1:5" hidden="1">
+    <row r="182" spans="1:5">
       <c r="A182" s="1" t="s">
         <v>641</v>
       </c>
@@ -7350,7 +7349,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="183" spans="1:5" hidden="1">
+    <row r="183" spans="1:5">
       <c r="A183" s="1" t="s">
         <v>645</v>
       </c>
@@ -7364,7 +7363,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="184" spans="1:5" hidden="1">
+    <row r="184" spans="1:5">
       <c r="A184" s="1" t="s">
         <v>649</v>
       </c>
@@ -7395,7 +7394,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="186" spans="1:5" hidden="1">
+    <row r="186" spans="1:5">
       <c r="A186" s="1" t="s">
         <v>655</v>
       </c>
@@ -7443,7 +7442,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="189" spans="1:5" hidden="1">
+    <row r="189" spans="1:5">
       <c r="A189" s="1" t="s">
         <v>663</v>
       </c>
@@ -7457,7 +7456,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="190" spans="1:5" hidden="1">
+    <row r="190" spans="1:5">
       <c r="A190" s="1" t="s">
         <v>667</v>
       </c>
@@ -7471,7 +7470,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="191" spans="1:5" hidden="1">
+    <row r="191" spans="1:5">
       <c r="A191" s="1" t="s">
         <v>671</v>
       </c>
@@ -7502,7 +7501,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="193" spans="1:5" hidden="1">
+    <row r="193" spans="1:5">
       <c r="A193" s="1" t="s">
         <v>677</v>
       </c>
@@ -7516,7 +7515,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="194" spans="1:5" hidden="1">
+    <row r="194" spans="1:5">
       <c r="A194" s="1" t="s">
         <v>681</v>
       </c>
@@ -7530,7 +7529,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="195" spans="1:5" hidden="1">
+    <row r="195" spans="1:5">
       <c r="A195" s="1" t="s">
         <v>685</v>
       </c>
@@ -7544,7 +7543,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="196" spans="1:5" hidden="1">
+    <row r="196" spans="1:5">
       <c r="A196" s="1" t="s">
         <v>689</v>
       </c>
@@ -7575,7 +7574,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="198" spans="1:5" hidden="1">
+    <row r="198" spans="1:5">
       <c r="A198" s="1" t="s">
         <v>695</v>
       </c>
@@ -7589,7 +7588,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="199" spans="1:5" hidden="1">
+    <row r="199" spans="1:5">
       <c r="A199" s="1" t="s">
         <v>699</v>
       </c>
@@ -7620,7 +7619,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="201" spans="1:5" hidden="1">
+    <row r="201" spans="1:5">
       <c r="A201" s="1" t="s">
         <v>705</v>
       </c>
@@ -7651,7 +7650,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="203" spans="1:5" hidden="1">
+    <row r="203" spans="1:5">
       <c r="A203" s="1" t="s">
         <v>711</v>
       </c>
@@ -7665,7 +7664,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="204" spans="1:5" hidden="1">
+    <row r="204" spans="1:5">
       <c r="A204" s="1" t="s">
         <v>715</v>
       </c>
@@ -7679,7 +7678,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="205" spans="1:5" hidden="1">
+    <row r="205" spans="1:5">
       <c r="A205" s="1" t="s">
         <v>719</v>
       </c>
@@ -7693,7 +7692,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="206" spans="1:5" hidden="1">
+    <row r="206" spans="1:5">
       <c r="A206" s="1" t="s">
         <v>723</v>
       </c>
@@ -7707,7 +7706,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="207" spans="1:5" hidden="1">
+    <row r="207" spans="1:5">
       <c r="A207" s="1" t="s">
         <v>727</v>
       </c>
@@ -7721,7 +7720,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="208" spans="1:5" hidden="1">
+    <row r="208" spans="1:5">
       <c r="A208" s="1" t="s">
         <v>731</v>
       </c>
@@ -7735,7 +7734,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="209" spans="1:5" hidden="1">
+    <row r="209" spans="1:5">
       <c r="A209" s="1" t="s">
         <v>735</v>
       </c>
@@ -7749,7 +7748,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="210" spans="1:5" hidden="1">
+    <row r="210" spans="1:5">
       <c r="A210" s="1" t="s">
         <v>739</v>
       </c>
@@ -7763,7 +7762,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="211" spans="1:5" hidden="1">
+    <row r="211" spans="1:5">
       <c r="A211" s="1" t="s">
         <v>743</v>
       </c>
@@ -7794,7 +7793,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="213" spans="1:5" hidden="1">
+    <row r="213" spans="1:5">
       <c r="A213" s="1" t="s">
         <v>749</v>
       </c>
@@ -7825,7 +7824,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="215" spans="1:5" hidden="1">
+    <row r="215" spans="1:5">
       <c r="A215" s="1" t="s">
         <v>755</v>
       </c>
@@ -7890,7 +7889,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="219" spans="1:5" hidden="1">
+    <row r="219" spans="1:5">
       <c r="A219" s="1" t="s">
         <v>765</v>
       </c>
@@ -7921,7 +7920,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="221" spans="1:5" hidden="1">
+    <row r="221" spans="1:5">
       <c r="A221" s="1" t="s">
         <v>771</v>
       </c>
@@ -7935,7 +7934,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="222" spans="1:5" hidden="1">
+    <row r="222" spans="1:5">
       <c r="A222" s="1" t="s">
         <v>775</v>
       </c>
@@ -7949,7 +7948,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="223" spans="1:5" hidden="1">
+    <row r="223" spans="1:5">
       <c r="A223" s="1" t="s">
         <v>779</v>
       </c>
@@ -7963,7 +7962,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="224" spans="1:5" hidden="1">
+    <row r="224" spans="1:5">
       <c r="A224" s="1" t="s">
         <v>783</v>
       </c>
@@ -7977,7 +7976,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="225" spans="1:5" hidden="1">
+    <row r="225" spans="1:5">
       <c r="A225" s="1" t="s">
         <v>787</v>
       </c>
@@ -7991,7 +7990,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="226" spans="1:5" hidden="1">
+    <row r="226" spans="1:5">
       <c r="A226" s="1" t="s">
         <v>791</v>
       </c>
@@ -8039,7 +8038,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="229" spans="1:5" hidden="1">
+    <row r="229" spans="1:5">
       <c r="A229" s="1" t="s">
         <v>799</v>
       </c>
@@ -8070,7 +8069,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="231" spans="1:5" hidden="1">
+    <row r="231" spans="1:5">
       <c r="A231" s="1" t="s">
         <v>805</v>
       </c>
@@ -8101,7 +8100,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="233" spans="1:5" hidden="1">
+    <row r="233" spans="1:5">
       <c r="A233" s="1" t="s">
         <v>811</v>
       </c>
@@ -8115,7 +8114,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="234" spans="1:5" hidden="1">
+    <row r="234" spans="1:5">
       <c r="A234" s="1" t="s">
         <v>815</v>
       </c>
@@ -8129,7 +8128,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="235" spans="1:5" hidden="1">
+    <row r="235" spans="1:5">
       <c r="A235" s="1" t="s">
         <v>819</v>
       </c>
@@ -8160,7 +8159,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="237" spans="1:5" hidden="1">
+    <row r="237" spans="1:5">
       <c r="A237" s="1" t="s">
         <v>825</v>
       </c>
@@ -8174,7 +8173,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="238" spans="1:5" hidden="1">
+    <row r="238" spans="1:5">
       <c r="A238" s="1" t="s">
         <v>829</v>
       </c>
@@ -8188,7 +8187,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="239" spans="1:5" hidden="1">
+    <row r="239" spans="1:5">
       <c r="A239" s="1" t="s">
         <v>833</v>
       </c>
@@ -8202,7 +8201,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="240" spans="1:5" hidden="1">
+    <row r="240" spans="1:5">
       <c r="A240" s="1" t="s">
         <v>837</v>
       </c>
@@ -8233,7 +8232,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="242" spans="1:5" hidden="1">
+    <row r="242" spans="1:5">
       <c r="A242" s="1" t="s">
         <v>843</v>
       </c>
@@ -8247,7 +8246,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="243" spans="1:5" hidden="1">
+    <row r="243" spans="1:5">
       <c r="A243" s="1" t="s">
         <v>847</v>
       </c>
@@ -8295,7 +8294,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="246" spans="1:5" hidden="1">
+    <row r="246" spans="1:5">
       <c r="A246" s="1" t="s">
         <v>855</v>
       </c>
@@ -8326,7 +8325,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="248" spans="1:5" hidden="1">
+    <row r="248" spans="1:5">
       <c r="A248" s="1" t="s">
         <v>861</v>
       </c>
@@ -8340,7 +8339,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="249" spans="1:5" hidden="1">
+    <row r="249" spans="1:5">
       <c r="A249" s="1" t="s">
         <v>865</v>
       </c>
@@ -8354,7 +8353,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="250" spans="1:5" hidden="1">
+    <row r="250" spans="1:5">
       <c r="A250" s="1" t="s">
         <v>869</v>
       </c>
@@ -8368,7 +8367,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="251" spans="1:5" hidden="1">
+    <row r="251" spans="1:5">
       <c r="A251" s="1" t="s">
         <v>873</v>
       </c>
@@ -8382,7 +8381,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="252" spans="1:5" hidden="1">
+    <row r="252" spans="1:5">
       <c r="A252" s="1" t="s">
         <v>877</v>
       </c>
@@ -8396,7 +8395,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="253" spans="1:5" hidden="1">
+    <row r="253" spans="1:5">
       <c r="A253" s="1" t="s">
         <v>881</v>
       </c>
@@ -8427,7 +8426,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="255" spans="1:5" hidden="1">
+    <row r="255" spans="1:5">
       <c r="A255" s="1" t="s">
         <v>887</v>
       </c>
@@ -8441,7 +8440,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="256" spans="1:5" hidden="1">
+    <row r="256" spans="1:5">
       <c r="A256" s="1" t="s">
         <v>891</v>
       </c>
@@ -8455,7 +8454,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="257" spans="1:5" hidden="1">
+    <row r="257" spans="1:5">
       <c r="A257" s="1" t="s">
         <v>895</v>
       </c>
@@ -8486,7 +8485,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="259" spans="1:5" hidden="1">
+    <row r="259" spans="1:5">
       <c r="A259" s="1" t="s">
         <v>901</v>
       </c>
@@ -8500,7 +8499,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="260" spans="1:5" hidden="1">
+    <row r="260" spans="1:5">
       <c r="A260" s="1" t="s">
         <v>905</v>
       </c>
@@ -8514,7 +8513,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="261" spans="1:5" hidden="1">
+    <row r="261" spans="1:5">
       <c r="A261" s="1" t="s">
         <v>909</v>
       </c>
@@ -8528,7 +8527,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="262" spans="1:5" hidden="1">
+    <row r="262" spans="1:5">
       <c r="A262" s="1" t="s">
         <v>913</v>
       </c>
@@ -8576,7 +8575,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="265" spans="1:5" hidden="1">
+    <row r="265" spans="1:5">
       <c r="A265" s="1" t="s">
         <v>921</v>
       </c>
@@ -8590,7 +8589,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="266" spans="1:5" hidden="1">
+    <row r="266" spans="1:5">
       <c r="A266" s="1" t="s">
         <v>925</v>
       </c>
@@ -8604,7 +8603,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="267" spans="1:5" hidden="1">
+    <row r="267" spans="1:5">
       <c r="A267" s="1" t="s">
         <v>929</v>
       </c>
@@ -8686,7 +8685,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="272" spans="1:5" hidden="1">
+    <row r="272" spans="1:5">
       <c r="A272" s="1" t="s">
         <v>941</v>
       </c>
@@ -8700,7 +8699,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="273" spans="1:5" hidden="1">
+    <row r="273" spans="1:5">
       <c r="A273" s="1" t="s">
         <v>945</v>
       </c>
@@ -8799,7 +8798,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="279" spans="1:5" hidden="1">
+    <row r="279" spans="1:5">
       <c r="A279" s="1" t="s">
         <v>959</v>
       </c>
@@ -8813,7 +8812,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="280" spans="1:5" hidden="1">
+    <row r="280" spans="1:5">
       <c r="A280" s="1" t="s">
         <v>963</v>
       </c>
@@ -8827,7 +8826,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="281" spans="1:5" hidden="1">
+    <row r="281" spans="1:5">
       <c r="A281" s="1" t="s">
         <v>967</v>
       </c>
@@ -8841,7 +8840,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="282" spans="1:5" hidden="1">
+    <row r="282" spans="1:5">
       <c r="A282" s="1" t="s">
         <v>971</v>
       </c>
@@ -8855,7 +8854,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="283" spans="1:5" hidden="1">
+    <row r="283" spans="1:5">
       <c r="A283" s="1" t="s">
         <v>975</v>
       </c>
@@ -8869,7 +8868,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="284" spans="1:5" hidden="1">
+    <row r="284" spans="1:5">
       <c r="A284" s="1" t="s">
         <v>979</v>
       </c>
@@ -8883,7 +8882,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="285" spans="1:5" hidden="1">
+    <row r="285" spans="1:5">
       <c r="A285" s="1" t="s">
         <v>983</v>
       </c>
@@ -8897,7 +8896,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="286" spans="1:5" hidden="1">
+    <row r="286" spans="1:5">
       <c r="A286" s="1" t="s">
         <v>987</v>
       </c>
@@ -8911,7 +8910,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="287" spans="1:5" hidden="1">
+    <row r="287" spans="1:5">
       <c r="A287" s="1" t="s">
         <v>991</v>
       </c>
@@ -8925,7 +8924,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="288" spans="1:5" hidden="1">
+    <row r="288" spans="1:5">
       <c r="A288" s="1" t="s">
         <v>995</v>
       </c>
@@ -8956,7 +8955,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="290" spans="1:5" hidden="1">
+    <row r="290" spans="1:5">
       <c r="A290" s="1" t="s">
         <v>1001</v>
       </c>
@@ -8970,7 +8969,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="291" spans="1:5" hidden="1">
+    <row r="291" spans="1:5">
       <c r="A291" s="1" t="s">
         <v>1005</v>
       </c>
@@ -8984,7 +8983,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="292" spans="1:5" hidden="1">
+    <row r="292" spans="1:5">
       <c r="A292" s="1" t="s">
         <v>1009</v>
       </c>
@@ -8998,7 +8997,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="293" spans="1:5" hidden="1">
+    <row r="293" spans="1:5">
       <c r="A293" s="1" t="s">
         <v>1013</v>
       </c>
@@ -9012,7 +9011,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="294" spans="1:5" hidden="1">
+    <row r="294" spans="1:5">
       <c r="A294" s="1" t="s">
         <v>1017</v>
       </c>
@@ -9043,7 +9042,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="296" spans="1:5" hidden="1">
+    <row r="296" spans="1:5">
       <c r="A296" s="1" t="s">
         <v>1023</v>
       </c>
@@ -9074,7 +9073,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="298" spans="1:5" hidden="1">
+    <row r="298" spans="1:5">
       <c r="A298" s="1" t="s">
         <v>1029</v>
       </c>
@@ -9105,7 +9104,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="300" spans="1:5" hidden="1">
+    <row r="300" spans="1:5">
       <c r="A300" s="1" t="s">
         <v>1035</v>
       </c>
@@ -9136,7 +9135,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="302" spans="1:5" hidden="1">
+    <row r="302" spans="1:5">
       <c r="A302" s="1" t="s">
         <v>1041</v>
       </c>
@@ -9150,7 +9149,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="303" spans="1:5" hidden="1">
+    <row r="303" spans="1:5">
       <c r="A303" s="1" t="s">
         <v>1045</v>
       </c>
@@ -9164,7 +9163,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="304" spans="1:5" hidden="1">
+    <row r="304" spans="1:5">
       <c r="A304" s="1" t="s">
         <v>1049</v>
       </c>
@@ -9178,7 +9177,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="305" spans="1:5" hidden="1">
+    <row r="305" spans="1:5">
       <c r="A305" s="1" t="s">
         <v>1053</v>
       </c>
@@ -9192,7 +9191,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="306" spans="1:5" hidden="1">
+    <row r="306" spans="1:5">
       <c r="A306" s="1" t="s">
         <v>1057</v>
       </c>
@@ -9223,7 +9222,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="308" spans="1:5" hidden="1">
+    <row r="308" spans="1:5">
       <c r="A308" s="1" t="s">
         <v>1063</v>
       </c>
@@ -9237,7 +9236,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="309" spans="1:5" hidden="1">
+    <row r="309" spans="1:5">
       <c r="A309" s="1" t="s">
         <v>1067</v>
       </c>
@@ -9251,7 +9250,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="310" spans="1:5" hidden="1">
+    <row r="310" spans="1:5">
       <c r="A310" s="1" t="s">
         <v>1071</v>
       </c>
@@ -9333,7 +9332,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="315" spans="1:5" hidden="1">
+    <row r="315" spans="1:5">
       <c r="A315" s="1" t="s">
         <v>1083</v>
       </c>
@@ -9347,7 +9346,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="316" spans="1:5" hidden="1">
+    <row r="316" spans="1:5">
       <c r="A316" s="1" t="s">
         <v>1087</v>
       </c>
@@ -9412,7 +9411,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="320" spans="1:5" hidden="1">
+    <row r="320" spans="1:5">
       <c r="A320" s="1" t="s">
         <v>1097</v>
       </c>
@@ -9426,7 +9425,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="321" spans="1:5" hidden="1">
+    <row r="321" spans="1:5">
       <c r="A321" s="1" t="s">
         <v>1101</v>
       </c>
@@ -9440,7 +9439,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="322" spans="1:5" hidden="1">
+    <row r="322" spans="1:5">
       <c r="A322" s="1" t="s">
         <v>1105</v>
       </c>
@@ -9573,7 +9572,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="330" spans="1:5" hidden="1">
+    <row r="330" spans="1:5">
       <c r="A330" s="1" t="s">
         <v>1123</v>
       </c>
@@ -9587,7 +9586,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="331" spans="1:5" hidden="1">
+    <row r="331" spans="1:5">
       <c r="A331" s="1" t="s">
         <v>1127</v>
       </c>
@@ -9601,7 +9600,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="332" spans="1:5" hidden="1">
+    <row r="332" spans="1:5">
       <c r="A332" s="1" t="s">
         <v>1131</v>
       </c>
@@ -9615,7 +9614,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="333" spans="1:5" hidden="1">
+    <row r="333" spans="1:5">
       <c r="A333" s="1" t="s">
         <v>1135</v>
       </c>
@@ -9629,7 +9628,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="334" spans="1:5" hidden="1">
+    <row r="334" spans="1:5">
       <c r="A334" s="1" t="s">
         <v>1139</v>
       </c>
@@ -9643,7 +9642,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="335" spans="1:5" hidden="1">
+    <row r="335" spans="1:5">
       <c r="A335" s="1" t="s">
         <v>1143</v>
       </c>
@@ -9708,7 +9707,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="339" spans="1:5" hidden="1">
+    <row r="339" spans="1:5">
       <c r="A339" s="1" t="s">
         <v>1153</v>
       </c>
@@ -9824,7 +9823,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="346" spans="1:5" hidden="1">
+    <row r="346" spans="1:5">
       <c r="A346" s="1" t="s">
         <v>1169</v>
       </c>
@@ -9889,7 +9888,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="350" spans="1:5" hidden="1">
+    <row r="350" spans="1:5">
       <c r="A350" s="1" t="s">
         <v>1179</v>
       </c>
@@ -9903,7 +9902,7 @@
         <v>1176</v>
       </c>
     </row>
-    <row r="351" spans="1:5" hidden="1">
+    <row r="351" spans="1:5">
       <c r="A351" s="1" t="s">
         <v>1183</v>
       </c>
@@ -9917,7 +9916,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="352" spans="1:5" hidden="1">
+    <row r="352" spans="1:5">
       <c r="A352" s="1" t="s">
         <v>1187</v>
       </c>
@@ -9982,7 +9981,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="356" spans="1:5" hidden="1">
+    <row r="356" spans="1:5">
       <c r="A356" s="1" t="s">
         <v>1197</v>
       </c>
@@ -9996,7 +9995,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="357" spans="1:5" hidden="1">
+    <row r="357" spans="1:5">
       <c r="A357" s="1" t="s">
         <v>1201</v>
       </c>
@@ -10010,7 +10009,7 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="358" spans="1:5" hidden="1">
+    <row r="358" spans="1:5">
       <c r="A358" s="1" t="s">
         <v>1205</v>
       </c>
@@ -10041,7 +10040,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="360" spans="1:5" hidden="1">
+    <row r="360" spans="1:5">
       <c r="A360" s="1" t="s">
         <v>1211</v>
       </c>
@@ -10055,7 +10054,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="361" spans="1:5" hidden="1">
+    <row r="361" spans="1:5">
       <c r="A361" s="1" t="s">
         <v>1215</v>
       </c>
@@ -10069,7 +10068,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="362" spans="1:5" hidden="1">
+    <row r="362" spans="1:5">
       <c r="A362" s="1" t="s">
         <v>1219</v>
       </c>
@@ -10083,7 +10082,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="363" spans="1:5" hidden="1">
+    <row r="363" spans="1:5">
       <c r="A363" s="1" t="s">
         <v>1223</v>
       </c>
@@ -10131,7 +10130,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="366" spans="1:5" hidden="1">
+    <row r="366" spans="1:5">
       <c r="A366" s="1" t="s">
         <v>1231</v>
       </c>
@@ -10145,7 +10144,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="367" spans="1:5" hidden="1">
+    <row r="367" spans="1:5">
       <c r="A367" s="1" t="s">
         <v>1235</v>
       </c>
@@ -10176,7 +10175,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="369" spans="1:5" hidden="1">
+    <row r="369" spans="1:5">
       <c r="A369" s="1" t="s">
         <v>1241</v>
       </c>
@@ -10207,7 +10206,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="371" spans="1:5" hidden="1">
+    <row r="371" spans="1:5">
       <c r="A371" s="1" t="s">
         <v>1247</v>
       </c>
@@ -10238,7 +10237,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="373" spans="1:5" hidden="1">
+    <row r="373" spans="1:5">
       <c r="A373" s="1" t="s">
         <v>1253</v>
       </c>
@@ -10269,7 +10268,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="375" spans="1:5" hidden="1">
+    <row r="375" spans="1:5">
       <c r="A375" s="1" t="s">
         <v>1259</v>
       </c>
@@ -10283,7 +10282,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="376" spans="1:5" hidden="1">
+    <row r="376" spans="1:5">
       <c r="A376" s="1" t="s">
         <v>1263</v>
       </c>
@@ -10297,7 +10296,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="377" spans="1:5" hidden="1">
+    <row r="377" spans="1:5">
       <c r="A377" s="1" t="s">
         <v>1267</v>
       </c>
@@ -10379,7 +10378,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="382" spans="1:5" hidden="1">
+    <row r="382" spans="1:5">
       <c r="A382" s="1" t="s">
         <v>1279</v>
       </c>
@@ -10410,7 +10409,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="384" spans="1:5" hidden="1">
+    <row r="384" spans="1:5">
       <c r="A384" s="1" t="s">
         <v>1285</v>
       </c>
@@ -10509,7 +10508,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="390" spans="1:5" hidden="1">
+    <row r="390" spans="1:5">
       <c r="A390" s="1" t="s">
         <v>1299</v>
       </c>
@@ -10523,7 +10522,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="391" spans="1:5" hidden="1">
+    <row r="391" spans="1:5">
       <c r="A391" s="1" t="s">
         <v>1303</v>
       </c>
@@ -10537,7 +10536,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="392" spans="1:5" hidden="1">
+    <row r="392" spans="1:5">
       <c r="A392" s="1" t="s">
         <v>1307</v>
       </c>
@@ -10568,7 +10567,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="394" spans="1:5" hidden="1">
+    <row r="394" spans="1:5">
       <c r="A394" s="1" t="s">
         <v>1313</v>
       </c>
@@ -10633,7 +10632,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="398" spans="1:5" hidden="1">
+    <row r="398" spans="1:5">
       <c r="A398" s="1" t="s">
         <v>1323</v>
       </c>
@@ -10664,7 +10663,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="400" spans="1:5" hidden="1">
+    <row r="400" spans="1:5">
       <c r="A400" s="1" t="s">
         <v>1329</v>
       </c>
@@ -10695,7 +10694,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="402" spans="1:5" hidden="1">
+    <row r="402" spans="1:5">
       <c r="A402" s="1" t="s">
         <v>1335</v>
       </c>
@@ -10709,7 +10708,7 @@
         <v>1332</v>
       </c>
     </row>
-    <row r="403" spans="1:5" hidden="1">
+    <row r="403" spans="1:5">
       <c r="A403" s="1" t="s">
         <v>1339</v>
       </c>
@@ -10774,7 +10773,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="407" spans="1:5" hidden="1">
+    <row r="407" spans="1:5">
       <c r="A407" s="1" t="s">
         <v>1349</v>
       </c>
@@ -10839,7 +10838,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="411" spans="1:5" hidden="1">
+    <row r="411" spans="1:5">
       <c r="A411" s="1" t="s">
         <v>1359</v>
       </c>
@@ -10853,7 +10852,7 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="412" spans="1:5" hidden="1">
+    <row r="412" spans="1:5">
       <c r="A412" s="1" t="s">
         <v>1363</v>
       </c>
@@ -10884,7 +10883,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="414" spans="1:5" hidden="1">
+    <row r="414" spans="1:5">
       <c r="A414" s="1" t="s">
         <v>1369</v>
       </c>
@@ -10898,7 +10897,7 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="415" spans="1:5" hidden="1">
+    <row r="415" spans="1:5">
       <c r="A415" s="1" t="s">
         <v>1373</v>
       </c>
@@ -11082,7 +11081,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="426" spans="1:5" hidden="1">
+    <row r="426" spans="1:5">
       <c r="A426" s="1" t="s">
         <v>1397</v>
       </c>
@@ -11096,7 +11095,7 @@
         <v>1394</v>
       </c>
     </row>
-    <row r="427" spans="1:5" hidden="1">
+    <row r="427" spans="1:5">
       <c r="A427" s="1" t="s">
         <v>1401</v>
       </c>
@@ -11110,7 +11109,7 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="428" spans="1:5" hidden="1">
+    <row r="428" spans="1:5">
       <c r="A428" s="1" t="s">
         <v>1405</v>
       </c>
@@ -11159,13 +11158,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B430" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="null"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>